<commit_message>
Alterado capitulo 4, subcapitulo testes de sistema
</commit_message>
<xml_diff>
--- a/Casos de Testes.xlsx
+++ b/Casos de Testes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8355"/>
+    <workbookView windowWidth="18345" windowHeight="11910"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60">
   <si>
     <t>ID</t>
   </si>
@@ -59,6 +59,141 @@
   </si>
   <si>
     <t>P7 - R. Arthur Portes, 101 - Vila Sao Joao</t>
+  </si>
+  <si>
+    <t>CT2</t>
+  </si>
+  <si>
+    <t>Cenário de Teste 2 :Esta validação tem por objetivo a definição de de 9 pontos atendidos pela Empresa 2 na Cidade de São José dos Campos- São Paulo. Sendo esses pontos compostos pela Origem e Destino que é o endereço da empresa e 9 pontos Intermediários</t>
+  </si>
+  <si>
+    <t>P0 - Estr. Mun. Martins Guimarães, 1050 - Vila Tesouro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P0 -&gt; P4 -&gt; P8-&gt; P5 -&gt; P1 -&gt;P7 -&gt; P6 -&gt; P3 -&gt; P2 -&gt;  P0 </t>
+  </si>
+  <si>
+    <t>P1 -  Av. São João, 2200 - Jardim das Colinas</t>
+  </si>
+  <si>
+    <t>P2 - Av. Dr. João Batista de Souza Soares, 3359 - Jardim Morumbi</t>
+  </si>
+  <si>
+    <t>P3 - Av. Cassiopeia, 591 - Jardim Satélite</t>
+  </si>
+  <si>
+    <t>P4 - Av. Pres. Juscelino Kubitschek, 6005</t>
+  </si>
+  <si>
+    <t>P5 - R. Claudino Pinto, 29 - Centro</t>
+  </si>
+  <si>
+    <t>P6 - Av. Andrômeda, 227 - Jardim Satélite</t>
+  </si>
+  <si>
+    <t>P7 - Av. Cassiano Ricardo, 1501 - Jardim Alvorada</t>
+  </si>
+  <si>
+    <t>P8 - Av. Nair Toledo de Mira, 4496 - Jardim Paulista</t>
+  </si>
+  <si>
+    <t>CT3</t>
+  </si>
+  <si>
+    <t>Cenário de Teste 3 :Esta validação tem por objetivo a definição de de 9 pontos atendidos pela Empresa 3 na Cidade de Taubaté- São Paulo. Sendo esses pontos compostos pela Origem e Destino que é o endereço da empresa e 9 pontos Intermediários</t>
+  </si>
+  <si>
+    <t>P0 - Estrada Municipal João Gadioli, 1330 - Quiririm</t>
+  </si>
+  <si>
+    <t>P0 -&gt; P6 -&gt; P4 -&gt; P2 -&gt; P7 -&gt; P3 -&gt; P8 -&gt; P5 -&gt; P1 -&gt; P0</t>
+  </si>
+  <si>
+    <t>P1 - Av. Dom Pedro I, 7181 - Res. Estoril</t>
+  </si>
+  <si>
+    <t>P2 - Av. Charles Schnneider, 1700 - Vila Costa</t>
+  </si>
+  <si>
+    <t>P3 -  Av. Professor Walter Taumaturgo, 1160 - Centro</t>
+  </si>
+  <si>
+    <t>P4 -  Av. Haroldo Mattos, 1780 - Parque Sr. do Bonfim,</t>
+  </si>
+  <si>
+    <t>P5 - Avenida Santa Cruz, 384 - Areão</t>
+  </si>
+  <si>
+    <t>P6 - Av. dos Imigrantes, 111 - Conj. Res. Quiririm,</t>
+  </si>
+  <si>
+    <t>P7 -  Av. Charles Schnneider, 420 - Parque Sr. do Bonfim</t>
+  </si>
+  <si>
+    <t>P8 - Av. Bandeirantes, 808 - Jardim Maria Augusta</t>
+  </si>
+  <si>
+    <t>CT4</t>
+  </si>
+  <si>
+    <t>Cenário de Teste 4 :Esta validação tem por objetivo a definição de de 7 pontos atendidos pela Empresa 4 na Cidade de Jacareí- São Paulo. Sendo esses pontos compostos pela Origem e Destino que é o endereço da empresa e 7 pontos Intermediários</t>
+  </si>
+  <si>
+    <t>P0 -Av. Getúlio Dorneles Vargas, 1390 - Jardim California</t>
+  </si>
+  <si>
+    <t>P0 -&gt;  P4 -&gt; P2 -&gt; P1 -&gt; P3 -&gt; P5 -&gt; P6 -&gt; P7 -&gt; P0</t>
+  </si>
+  <si>
+    <t>P1 - Av. São João, 109 - São João</t>
+  </si>
+  <si>
+    <t>P2 -R. José Benedito Duarte, 88 - Parque Itamarati</t>
+  </si>
+  <si>
+    <t>P3 - Av. Pereira Campos, 291 - Jardim Didinha,</t>
+  </si>
+  <si>
+    <t>P4 - Av. Getúlio Dorneles Vargas, 1591 - Jardim California,</t>
+  </si>
+  <si>
+    <t>P5 - Av. Sebastião Lopes, 42 - Jardim Nova Esperança</t>
+  </si>
+  <si>
+    <t>P6 -Avenida das Letras, Loteamento Villa Branca</t>
+  </si>
+  <si>
+    <t>P7 - Av. São Jorge, 2010 - Jardim Santa Marina</t>
+  </si>
+  <si>
+    <t>CT5</t>
+  </si>
+  <si>
+    <t>Cenário de Teste 5 :Esta validação tem por objetivo a definição de de 6 pontos atendidos pela Empresa 4 na Cidade de Caraguatatuba- São Paulo. Sendo esses pontos compostos pela Origem e Destino que é o endereço da empresa e 6 pontos Intermediários</t>
+  </si>
+  <si>
+    <t>P0 - Rua Hermes da Fonseca, 217 - Poiares</t>
+  </si>
+  <si>
+    <t>P0 -&gt; P4 -&gt; P5 -&gt; P6 -&gt; P3 -&gt; P1 -&gt; P2  -&gt; P0</t>
+  </si>
+  <si>
+    <t>P1 - Av. Prisciliana de Castilho, 840 - Caputera</t>
+  </si>
+  <si>
+    <t>P2 - R. Silvio de Oliveira - Praia das Palmeiras</t>
+  </si>
+  <si>
+    <t>P3 - Av. Pres. Campos Sales, 297 - Jaraguazinho,</t>
+  </si>
+  <si>
+    <t>P4 - R. João Café Filho, 141 - Poiares</t>
+  </si>
+  <si>
+    <t>P5 - R. Maria Augusta dos Anjos, 96 - Tingá</t>
+  </si>
+  <si>
+    <t>P6 - Av. Mato Grosso, 838 - Indaiá</t>
   </si>
 </sst>
 </file>
@@ -66,10 +201,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -96,7 +231,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -110,6 +245,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -126,8 +268,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,7 +292,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -164,14 +307,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,16 +329,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,6 +345,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,14 +366,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -247,187 +382,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,11 +643,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,8 +661,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,17 +682,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -581,21 +731,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -607,22 +742,22 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -631,122 +766,122 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -776,6 +911,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1096,10 +1243,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:D10"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1200,11 +1347,399 @@
       </c>
       <c r="D10" s="8"/>
     </row>
+    <row r="12" ht="30" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" ht="30" spans="1:4">
+      <c r="A13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" ht="30" spans="1:4">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" ht="45" spans="1:4">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" ht="30" spans="1:4">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" ht="30" spans="1:4">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="13"/>
+    </row>
+    <row r="18" ht="30" spans="1:4">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" ht="30" spans="1:4">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" ht="30" spans="1:4">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" ht="30" spans="1:4">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" ht="30" spans="1:4">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="13"/>
+    </row>
+    <row r="24" ht="30" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" ht="30" spans="1:4">
+      <c r="A25" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" ht="30" spans="1:4">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" ht="30" spans="1:4">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" ht="30" spans="1:4">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" ht="30" spans="1:4">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" ht="30" spans="1:4">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" ht="30" spans="1:4">
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" ht="30" spans="1:4">
+      <c r="A32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" ht="30" spans="1:4">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" ht="30" spans="1:4">
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="36" ht="30" spans="1:4">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" ht="30" spans="1:4">
+      <c r="A37" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="13"/>
+    </row>
+    <row r="39" ht="30" spans="1:4">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="13"/>
+    </row>
+    <row r="40" ht="30" spans="1:4">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="13"/>
+    </row>
+    <row r="41" ht="30" spans="1:4">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="13"/>
+    </row>
+    <row r="42" ht="30" spans="1:4">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="13"/>
+    </row>
+    <row r="43" ht="30" spans="1:4">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="13"/>
+    </row>
+    <row r="44" ht="30" spans="1:4">
+      <c r="A44" s="10"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="13"/>
+    </row>
+    <row r="45" ht="30" spans="1:4">
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="13"/>
+    </row>
+    <row r="47" ht="30" spans="1:4">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" ht="30" spans="1:4">
+      <c r="A48" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" ht="30" spans="1:4">
+      <c r="A49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="13"/>
+    </row>
+    <row r="50" ht="30" spans="1:4">
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" s="13"/>
+    </row>
+    <row r="51" ht="30" spans="1:4">
+      <c r="A51" s="10"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="13"/>
+    </row>
+    <row r="52" ht="30" spans="1:4">
+      <c r="A52" s="10"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="13"/>
+    </row>
+    <row r="53" ht="30" spans="1:4">
+      <c r="A53" s="10"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D53" s="13"/>
+    </row>
+    <row r="54" ht="30" spans="1:4">
+      <c r="A54" s="10"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" s="13"/>
+    </row>
+    <row r="55" ht="30" spans="1:4">
+      <c r="A55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="15">
     <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="A25:A34"/>
+    <mergeCell ref="A37:A45"/>
+    <mergeCell ref="A48:A55"/>
     <mergeCell ref="B2:B10"/>
+    <mergeCell ref="B13:B22"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="B37:B45"/>
+    <mergeCell ref="B48:B55"/>
     <mergeCell ref="D2:D10"/>
+    <mergeCell ref="D13:D22"/>
+    <mergeCell ref="D25:D34"/>
+    <mergeCell ref="D37:D45"/>
+    <mergeCell ref="D48:D55"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Realizada ultimaas correções | apresentação quase pronta | pdf Final gerado
</commit_message>
<xml_diff>
--- a/Casos de Testes.xlsx
+++ b/Casos de Testes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18345" windowHeight="11910"/>
+    <workbookView windowWidth="20385" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <t>CT1</t>
   </si>
   <si>
-    <t>Cenário de Teste 1 :Esta validação tem por objetivo a definição de de 5 pontos atendidos pela Empresa 1 na Cidade de Caçapava- São Paulo. Sendo esses pontos compostos pela Origem e Destino que é o endereço da empresa e 7 pontos Intermediários</t>
+    <t>Cenário de Teste 1 :Esta validação tem por objetivo a definição de de 7 pontos atendidos pela Empresa 1 na Cidade de Caçapava- São Paulo. Sendo esses pontos compostos pela Origem e Destino que é o endereço da empresa e 7 pontos Intermediários</t>
   </si>
   <si>
     <t>P0 - R. Ver. Geraldo Nogueira da Silva, 1000 - Res. Terras do Vale</t>
@@ -202,9 +202,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -224,14 +224,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,13 +267,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -260,6 +275,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -268,9 +329,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,29 +345,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -321,22 +359,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -344,28 +366,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -382,187 +382,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,15 +634,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -662,7 +653,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -678,6 +669,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -723,10 +725,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -742,142 +742,142 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1245,8 +1245,8 @@
   <sheetPr/>
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>

</xml_diff>